<commit_message>
update group info in contract_info.xlsx
</commit_message>
<xml_diff>
--- a/group_info.xlsx
+++ b/group_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jolyon Jian\Desktop\contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5AF753-4AE0-4FA4-A782-65D85CDE6251}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765DAD2F-160C-4110-8E81-327AAD43DFEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35835" yWindow="495" windowWidth="51195" windowHeight="26595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="522">
   <si>
     <t>备注</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1457,11 +1457,227 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>侧链Ronin桥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Axie Infinity: Ronin Bridge	</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenSea: Seaport 1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kraken 5 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Binance: Contract 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MMM BSC 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Polygon (Matic): Bridge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bridge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	StrongBlock: Service &amp; Kyber Network: KNC Token 代码完全一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代理 &amp; 所有权管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有权管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	 KOK PLAY: KOK Token &amp; Davinci Coin 代码完全一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	TRON: Old TRX Token &amp; BFX (BFX)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	1inch v3/1inch v4: Router/1inch Network v2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poloniex 2 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenSea: Registry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Registry</t>
+  </si>
+  <si>
+    <t>HEX.com: HEX Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bittrex 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fork split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exchange Proxy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proxy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PFeast (PFET) 未公开源码 反编译失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sweeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bittrex: Controller &amp; </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gemini 4 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENS: Old Registrar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Registrar</t>
+  </si>
+  <si>
+    <t>Bitstamp 2 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WorldUnitedCoins (WUC)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enjin Coin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EasyClub.live 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baer Chain: BRC Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cronos Coin: CRO Token &amp; Coti: COTI Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Million.Money</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Auction</t>
+  </si>
+  <si>
+    <t>CryptoKitties: Sales Auction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrueUSD: TUSD Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Axie Infinity: SLP Token &amp; Axie Infinity: AXS Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WENI (WENI) &amp; Serum: SRM Token &amp; Ultra: UOS Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POCC (POCC) &amp; ProofOfContributionToken (POCT)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eth2Dai: Old Contract/OasisDEX/OasisDex: Old Contract/OasisDex: Old Contract 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Synthetix: Proxy SNX Token/Synthetix: Proxy sUSD Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kraken: Deployer 2 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Golem Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status Network Token/Status: Token Sale 完全一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wintermute 1 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATB Banknote (ATB) 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码很短 没有太大相关性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molecular Future Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	Aave: AAVE Token/Uniswap: Token Distributor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exchange v3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biigo2 未公开源码 反编译获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Binance: BNB Token/PlexCoin (PLX)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1521,7 +1737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1540,6 +1756,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1846,15 +2068,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E432"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D451" sqref="D451"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.875" customWidth="1"/>
+    <col min="3" max="3" width="18" style="2" customWidth="1"/>
+    <col min="4" max="4" width="79.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="9" style="5"/>
   </cols>
   <sheetData>
@@ -1872,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1898,7 +2120,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1912,7 +2134,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +2162,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1954,7 +2176,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1982,7 +2204,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -2038,7 +2260,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -2052,7 +2274,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -2122,7 +2344,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2150,7 +2372,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -2200,10 +2422,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>465</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2220,20 +2442,32 @@
         <v>464</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="6">
         <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2243,13 +2477,25 @@
       <c r="B29" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="6">
         <v>13</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -2259,6 +2505,12 @@
       <c r="B31" s="6">
         <v>1</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -2267,448 +2519,784 @@
       <c r="B32" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B41" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B42" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B43" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B45" s="6">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B46" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B48" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B50" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B52" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B53" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B54" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B55" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B56" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B57" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B58" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B59" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B60" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B61" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B62" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B63" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B64" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B65" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B66" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B68" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B69" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B70" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B71" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C71" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B72" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B73" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B74" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B75" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B76" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B77" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B78" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B79" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B80" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B81" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C81" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B82" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B83" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B84" s="6">
         <v>28</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B85" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C85" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B86" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B87" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C87" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>90</v>
       </c>
@@ -2716,7 +3304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>91</v>
       </c>
@@ -2724,7 +3312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>92</v>
       </c>
@@ -2732,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>93</v>
       </c>
@@ -2740,7 +3328,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>94</v>
       </c>
@@ -2748,7 +3336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -2756,7 +3344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -2764,7 +3352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -2772,7 +3360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>98</v>
       </c>
@@ -2844,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>107</v>
       </c>
@@ -2860,7 +3448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>109</v>
       </c>
@@ -2868,7 +3456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>110</v>
       </c>
@@ -2876,7 +3464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>111</v>
       </c>
@@ -2900,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>114</v>
       </c>
@@ -2908,7 +3496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>115</v>
       </c>
@@ -2932,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>118</v>
       </c>
@@ -2972,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>123</v>
       </c>
@@ -2980,7 +3568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>124</v>
       </c>
@@ -2988,7 +3576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>125</v>
       </c>
@@ -2996,7 +3584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>126</v>
       </c>
@@ -3028,7 +3616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>130</v>
       </c>
@@ -3068,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>135</v>
       </c>
@@ -3100,7 +3688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>139</v>
       </c>
@@ -3116,7 +3704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>141</v>
       </c>
@@ -3124,7 +3712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>142</v>
       </c>
@@ -3140,7 +3728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>144</v>
       </c>
@@ -3148,7 +3736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>145</v>
       </c>
@@ -3172,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>148</v>
       </c>
@@ -3180,7 +3768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -3188,7 +3776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>150</v>
       </c>
@@ -3212,7 +3800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>153</v>
       </c>
@@ -3220,7 +3808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>154</v>
       </c>
@@ -3268,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>160</v>
       </c>
@@ -3276,7 +3864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>161</v>
       </c>
@@ -3284,7 +3872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>162</v>
       </c>
@@ -3308,7 +3896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>165</v>
       </c>
@@ -3324,7 +3912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>167</v>
       </c>
@@ -3348,7 +3936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>170</v>
       </c>
@@ -3380,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>174</v>
       </c>
@@ -3388,7 +3976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>175</v>
       </c>
@@ -3396,7 +3984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>176</v>
       </c>
@@ -3436,7 +4024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>181</v>
       </c>
@@ -3452,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>183</v>
       </c>
@@ -3468,7 +4056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>185</v>
       </c>
@@ -3508,7 +4096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>190</v>
       </c>
@@ -3516,7 +4104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>191</v>
       </c>
@@ -3548,7 +4136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>195</v>
       </c>
@@ -3564,7 +4152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>197</v>
       </c>
@@ -3572,7 +4160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>198</v>
       </c>
@@ -3596,7 +4184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>201</v>
       </c>
@@ -3604,7 +4192,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>202</v>
       </c>
@@ -3620,7 +4208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>204</v>
       </c>
@@ -3692,7 +4280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>213</v>
       </c>
@@ -3700,7 +4288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
         <v>214</v>
       </c>
@@ -3708,7 +4296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>215</v>
       </c>
@@ -3716,7 +4304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>216</v>
       </c>
@@ -3740,7 +4328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>219</v>
       </c>
@@ -3756,7 +4344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>221</v>
       </c>
@@ -3820,7 +4408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
         <v>229</v>
       </c>
@@ -3828,7 +4416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
         <v>230</v>
       </c>
@@ -3860,7 +4448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
         <v>234</v>
       </c>
@@ -3868,7 +4456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
         <v>235</v>
       </c>
@@ -3876,7 +4464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
         <v>236</v>
       </c>
@@ -3940,7 +4528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
         <v>244</v>
       </c>
@@ -3948,7 +4536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>245</v>
       </c>
@@ -3956,7 +4544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
         <v>246</v>
       </c>
@@ -3988,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
         <v>250</v>
       </c>
@@ -4028,7 +4616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
         <v>255</v>
       </c>
@@ -4084,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
         <v>262</v>
       </c>
@@ -4100,7 +4688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
         <v>264</v>
       </c>
@@ -4140,7 +4728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
         <v>269</v>
       </c>
@@ -4156,7 +4744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
         <v>271</v>
       </c>
@@ -4196,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="2" t="s">
         <v>276</v>
       </c>
@@ -4260,7 +4848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
         <v>284</v>
       </c>
@@ -4284,7 +4872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
         <v>287</v>
       </c>
@@ -4292,7 +4880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="2" t="s">
         <v>288</v>
       </c>
@@ -4324,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" s="2" t="s">
         <v>292</v>
       </c>
@@ -4380,7 +4968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="2" t="s">
         <v>299</v>
       </c>
@@ -4412,7 +5000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="2" t="s">
         <v>303</v>
       </c>
@@ -4500,7 +5088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="2" t="s">
         <v>314</v>
       </c>
@@ -4524,7 +5112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="2" t="s">
         <v>317</v>
       </c>
@@ -4548,7 +5136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" s="2" t="s">
         <v>320</v>
       </c>
@@ -4596,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="2" t="s">
         <v>326</v>
       </c>
@@ -4644,7 +5232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="2" t="s">
         <v>332</v>
       </c>
@@ -4716,7 +5304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="2" t="s">
         <v>341</v>
       </c>
@@ -4724,7 +5312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="340" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="2" t="s">
         <v>342</v>
       </c>
@@ -4852,7 +5440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" s="2" t="s">
         <v>358</v>
       </c>
@@ -4884,7 +5472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="2" t="s">
         <v>362</v>
       </c>
@@ -4956,7 +5544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" s="2" t="s">
         <v>371</v>
       </c>
@@ -4996,7 +5584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" s="2" t="s">
         <v>376</v>
       </c>
@@ -5324,7 +5912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" s="2" t="s">
         <v>417</v>
       </c>
@@ -5469,10 +6057,31 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D432" xr:uid="{04541F0E-5A7C-482F-903C-CC944D3CA814}">
+  <autoFilter ref="A1:D432" xr:uid="{B388CE93-5F50-4019-BD29-E88D4941BFDD}">
     <filterColumn colId="1">
       <filters>
+        <filter val="10"/>
+        <filter val="11"/>
+        <filter val="13"/>
+        <filter val="14"/>
+        <filter val="15"/>
+        <filter val="17"/>
+        <filter val="18"/>
+        <filter val="2"/>
+        <filter val="20"/>
+        <filter val="23"/>
+        <filter val="25"/>
+        <filter val="27"/>
+        <filter val="28"/>
+        <filter val="3"/>
+        <filter val="31"/>
         <filter val="35"/>
+        <filter val="4"/>
+        <filter val="5"/>
+        <filter val="6"/>
+        <filter val="7"/>
+        <filter val="8"/>
+        <filter val="9"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>